<commit_message>
2nd Phase of experiments
</commit_message>
<xml_diff>
--- a/Adult Income/model_perf_metrics_merged.xlsx
+++ b/Adult Income/model_perf_metrics_merged.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dideu\OneDrive\Documents\DDB\thesis\Thesis_Project\Adult Income\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7D5BF2-6FD6-4E03-98E7-291959D9728F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975E91C7-4578-4C21-8BF6-8F7492A17295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Model</t>
   </si>
@@ -161,13 +174,16 @@
   </si>
   <si>
     <t>LR _25000_2</t>
+  </si>
+  <si>
+    <t>Added_cf_num</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +195,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,11 +240,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="A3" sqref="A3:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,9 +559,10 @@
     <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,8 +584,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -579,7 +608,7 @@
         <v>0.7637742563211658</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -601,8 +630,12 @@
       <c r="G3">
         <v>30133</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3">
+        <f>G3-27133</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -624,8 +657,12 @@
       <c r="G4">
         <v>52133</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4">
+        <f t="shared" ref="H4:H42" si="0">G4-27133</f>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -647,8 +684,12 @@
       <c r="G5">
         <v>42133</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -670,8 +711,12 @@
       <c r="G6">
         <v>27633</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -693,8 +738,12 @@
       <c r="G7">
         <v>29133</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -716,8 +765,12 @@
       <c r="G8">
         <v>37133</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -739,8 +792,12 @@
       <c r="G9">
         <v>27633</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -762,8 +819,12 @@
       <c r="G10">
         <v>29633</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -785,8 +846,12 @@
       <c r="G11">
         <v>30133</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -808,8 +873,12 @@
       <c r="G12">
         <v>28633</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -831,8 +900,12 @@
       <c r="G13">
         <v>32133</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -854,8 +927,12 @@
       <c r="G14">
         <v>27133</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -877,8 +954,12 @@
       <c r="G15">
         <v>27233</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -900,8 +981,12 @@
       <c r="G16">
         <v>27333</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -923,8 +1008,12 @@
       <c r="G17">
         <v>27433</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -946,8 +1035,12 @@
       <c r="G18">
         <v>33133</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -969,8 +1062,12 @@
       <c r="G19">
         <v>27633</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -992,8 +1089,12 @@
       <c r="G20">
         <v>28133</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1015,8 +1116,12 @@
       <c r="G21">
         <v>28133</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1038,8 +1143,12 @@
       <c r="G22">
         <v>42133</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1061,8 +1170,12 @@
       <c r="G23">
         <v>28133</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1084,8 +1197,12 @@
       <c r="G24">
         <v>29133</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1107,8 +1224,12 @@
       <c r="G25">
         <v>29633</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1130,8 +1251,12 @@
       <c r="G26">
         <v>32133</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1153,8 +1278,12 @@
       <c r="G27">
         <v>32133</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1176,8 +1305,12 @@
       <c r="G28">
         <v>32133</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1199,8 +1332,12 @@
       <c r="G29">
         <v>32133</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1222,8 +1359,12 @@
       <c r="G30">
         <v>32133</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1245,8 +1386,12 @@
       <c r="G31">
         <v>37133</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -1268,8 +1413,12 @@
       <c r="G32">
         <v>37133</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1291,8 +1440,12 @@
       <c r="G33">
         <v>37133</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1314,8 +1467,12 @@
       <c r="G34">
         <v>37131</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>9998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1337,8 +1494,12 @@
       <c r="G35">
         <v>47133</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -1360,8 +1521,12 @@
       <c r="G36">
         <v>52133</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -1383,8 +1548,12 @@
       <c r="G37">
         <v>77133</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -1406,8 +1575,12 @@
       <c r="G38">
         <v>47133</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1429,8 +1602,12 @@
       <c r="G39">
         <v>67133</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -1452,8 +1629,12 @@
       <c r="G40">
         <v>57133</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -1475,8 +1656,12 @@
       <c r="G41">
         <v>77120</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>49987</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -1497,6 +1682,10 @@
       </c>
       <c r="G42">
         <v>126923</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>99790</v>
       </c>
     </row>
   </sheetData>
@@ -1504,5 +1693,6 @@
     <sortCondition descending="1" ref="E1:E43"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>